<commit_message>
Finalized review of station list.
</commit_message>
<xml_diff>
--- a/StationsToLocate/FinalList/Additional_LASAR_Stations.xlsx
+++ b/StationsToLocate/FinalList/Additional_LASAR_Stations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24915" windowHeight="12840"/>
+    <workbookView xWindow="15000" yWindow="450" windowWidth="10170" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="updated_field_names" sheetId="3" r:id="rId1"/>
@@ -12,7 +12,9 @@
     <sheet name="needs_review" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">updated_field_names!$A$1:$P$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">all_stations!$A$1:$V$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">needs_review!$A$1:$W$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">updated_field_names!$A$1:$R$45</definedName>
     <definedName name="_xlnm.Database">all_stations!$A$1:$V$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="162">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -430,24 +432,15 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Further Review Needed</t>
-  </si>
-  <si>
     <t>Most likely NF of Middle Fork Willamette</t>
   </si>
   <si>
-    <t>Station located on the wrong branch</t>
-  </si>
-  <si>
     <t>Potential Digitization</t>
   </si>
   <si>
     <t>Stream present in NHD, not DEQ streams.</t>
   </si>
   <si>
-    <t>No stream names to match off of</t>
-  </si>
-  <si>
     <t>DEQ streams not well delineated. NHD is better</t>
   </si>
   <si>
@@ -491,6 +484,30 @@
   </si>
   <si>
     <t>LLID</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Longitude is wrong. Could be re-located using description.</t>
+  </si>
+  <si>
+    <t>Likely Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not a surface water site. Came up because it has "SW" in the address. </t>
+  </si>
+  <si>
+    <t>AGENCY</t>
+  </si>
+  <si>
+    <t>AGENCY_ID</t>
+  </si>
+  <si>
+    <t>Oregon Department of Environmental Quality</t>
+  </si>
+  <si>
+    <t>ODEQ</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1333,17 +1350,19 @@
     <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.7109375" style="1" customWidth="1"/>
-    <col min="9" max="11" width="19.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="83.7109375" style="1" customWidth="1"/>
+    <col min="11" max="13" width="19.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,49 +1370,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1409,35 +1434,41 @@
       <c r="F2" s="2">
         <v>32.265093441499999</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="1">
         <v>36445</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2">
+      <c r="K2" s="2">
         <v>45.692309999999999</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L2" s="2">
         <v>-118.73502000000001</v>
       </c>
-      <c r="K2" s="2">
+      <c r="M2" s="2">
         <v>351</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1453,35 +1484,41 @@
       <c r="F3" s="2">
         <v>301.80591385700001</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" s="1">
         <v>12015</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="2">
+      <c r="K3" s="2">
         <v>45.784771999999997</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>-119.341281</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>170</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1">
         <v>2</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1497,35 +1534,41 @@
       <c r="F4" s="2">
         <v>581.89186180800004</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="1">
         <v>10708</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="2">
+      <c r="K4" s="2">
         <v>45.739806000000002</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>-120.023139</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>113</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="1">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1541,38 +1584,44 @@
       <c r="F5" s="2">
         <v>655.25162609200004</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" s="1">
         <v>34086</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="2">
+      <c r="K5" s="2">
         <v>45.389099999999999</v>
       </c>
-      <c r="J5" s="2">
+      <c r="L5" s="2">
         <v>-121.93767</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>716</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <v>4</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="P5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="P5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>154</v>
+      </c>
+      <c r="R5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1588,35 +1637,41 @@
       <c r="F6" s="2">
         <v>-419.08513926299997</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="1">
         <v>28010</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="2">
+      <c r="K6" s="2">
         <v>43.725999999999999</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>-122.4359</v>
       </c>
-      <c r="K6" s="2">
+      <c r="M6" s="2">
         <v>378</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="1">
         <v>5</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1632,35 +1687,41 @@
       <c r="F7" s="2">
         <v>354.61531665400003</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="1">
         <v>28608</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="2">
+      <c r="K7" s="2">
         <v>43.720970000000001</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>-122.43753</v>
       </c>
-      <c r="K7" s="2">
+      <c r="M7" s="2">
         <v>376</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="1">
         <v>6</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1676,35 +1737,41 @@
       <c r="F8" s="2">
         <v>-108.473015166</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="1">
         <v>10908</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="2">
+      <c r="K8" s="2">
         <v>43.740443999999997</v>
       </c>
-      <c r="J8" s="2">
+      <c r="L8" s="2">
         <v>-122.458611</v>
       </c>
-      <c r="K8" s="2">
+      <c r="M8" s="2">
         <v>355</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="1">
         <v>7</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:18">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1720,35 +1787,41 @@
       <c r="F9" s="2">
         <v>-366.25276947200001</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I9" s="1">
         <v>37318</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="2">
+      <c r="K9" s="2">
         <v>43.788705999999998</v>
       </c>
-      <c r="J9" s="2">
+      <c r="L9" s="2">
         <v>-122.461831</v>
       </c>
-      <c r="K9" s="2">
+      <c r="M9" s="2">
         <v>349</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="1">
         <v>8</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:18">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1764,35 +1837,41 @@
       <c r="F10" s="2">
         <v>120.319726907</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" s="1">
         <v>37317</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="2">
+      <c r="K10" s="2">
         <v>43.757106</v>
       </c>
-      <c r="J10" s="2">
+      <c r="L10" s="2">
         <v>-122.49672200000001</v>
       </c>
-      <c r="K10" s="2">
+      <c r="M10" s="2">
         <v>331</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="1">
         <v>9</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:18">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1808,38 +1887,44 @@
       <c r="F11" s="2">
         <v>75.777605241700002</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" s="1">
         <v>10913</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="2">
+      <c r="K11" s="2">
         <v>43.758944</v>
       </c>
-      <c r="J11" s="2">
+      <c r="L11" s="2">
         <v>-122.523556</v>
       </c>
-      <c r="K11" s="2">
+      <c r="M11" s="2">
         <v>315</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="1">
         <v>10</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>156</v>
+      </c>
+      <c r="R11" t="s">
         <v>136</v>
       </c>
-      <c r="P11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1855,35 +1940,41 @@
       <c r="F12" s="2">
         <v>204.27260615500001</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I12" s="1">
         <v>10668</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I12" s="2">
+      <c r="K12" s="2">
         <v>43.755222000000003</v>
       </c>
-      <c r="J12" s="2">
+      <c r="L12" s="2">
         <v>-122.526444</v>
       </c>
-      <c r="K12" s="2">
+      <c r="M12" s="2">
         <v>317</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="1">
         <v>11</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:18">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1899,35 +1990,41 @@
       <c r="F13" s="2">
         <v>163.02957825799999</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" s="1">
         <v>11375</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="2">
+      <c r="K13" s="2">
         <v>42.659360999999997</v>
       </c>
-      <c r="J13" s="2">
+      <c r="L13" s="2">
         <v>-122.698944</v>
       </c>
-      <c r="K13" s="2">
+      <c r="M13" s="2">
         <v>466</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="1">
         <v>12</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:18">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1943,35 +2040,41 @@
       <c r="F14" s="2">
         <v>35.990392590299997</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I14" s="1">
         <v>37308</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="2">
+      <c r="K14" s="2">
         <v>43.978009</v>
       </c>
-      <c r="J14" s="2">
+      <c r="L14" s="2">
         <v>-122.748783</v>
       </c>
-      <c r="K14" s="2">
+      <c r="M14" s="2">
         <v>232</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="1">
         <v>13</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:18">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1987,38 +2090,44 @@
       <c r="F15" s="2">
         <v>4914.3600231999999</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15" s="1">
         <v>37310</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="2">
+      <c r="K15" s="2">
         <v>43.926768000000003</v>
       </c>
-      <c r="J15" s="2">
+      <c r="L15" s="2">
         <v>-122.784783</v>
       </c>
-      <c r="K15" s="2">
+      <c r="M15" s="2">
         <v>232</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="1">
         <v>14</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="P15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2034,38 +2143,44 @@
       <c r="F16" s="2">
         <v>2857.6041715400002</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" s="1">
         <v>37309</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="2">
+      <c r="K16" s="2">
         <v>43.921047999999999</v>
       </c>
-      <c r="J16" s="2">
+      <c r="L16" s="2">
         <v>-122.786142</v>
       </c>
-      <c r="K16" s="2">
+      <c r="M16" s="2">
         <v>220</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="1">
         <v>15</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="P16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2081,35 +2196,41 @@
       <c r="F17" s="2">
         <v>163.39601961899999</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" s="1">
         <v>37312</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="2">
+      <c r="K17" s="2">
         <v>43.925148</v>
       </c>
-      <c r="J17" s="2">
+      <c r="L17" s="2">
         <v>-122.81068399999999</v>
       </c>
-      <c r="K17" s="2">
+      <c r="M17" s="2">
         <v>196</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="1">
         <v>17</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:18">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2125,35 +2246,41 @@
       <c r="F18" s="2">
         <v>42.778447677700001</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I18" s="1">
         <v>37299</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="2">
+      <c r="K18" s="2">
         <v>43.965007999999997</v>
       </c>
-      <c r="J18" s="2">
+      <c r="L18" s="2">
         <v>-122.849777</v>
       </c>
-      <c r="K18" s="2">
+      <c r="M18" s="2">
         <v>177</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="1">
         <v>18</v>
       </c>
-      <c r="N18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:18">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2169,38 +2296,44 @@
       <c r="F19" s="2">
         <v>1670.9214633199999</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="1">
         <v>35348</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="2">
+      <c r="K19" s="2">
         <v>45.448680000000003</v>
       </c>
-      <c r="J19" s="2">
+      <c r="L19" s="2">
         <v>-122.90025</v>
       </c>
-      <c r="K19" s="2">
+      <c r="M19" s="2">
         <v>91</v>
       </c>
-      <c r="L19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="1">
         <v>19</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="P19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="P19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>154</v>
+      </c>
+      <c r="R19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2216,35 +2349,41 @@
       <c r="F20" s="2">
         <v>54.1944730142</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I20" s="1">
         <v>37302</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="2">
+      <c r="K20" s="2">
         <v>43.996948000000003</v>
       </c>
-      <c r="J20" s="2">
+      <c r="L20" s="2">
         <v>-122.90402</v>
       </c>
-      <c r="K20" s="2">
+      <c r="M20" s="2">
         <v>163</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="1">
         <v>20</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:18">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2260,35 +2399,41 @@
       <c r="F21" s="2">
         <v>73.680022717900002</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I21" s="1">
         <v>37316</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="2">
+      <c r="K21" s="2">
         <v>44.000298000000001</v>
       </c>
-      <c r="J21" s="2">
+      <c r="L21" s="2">
         <v>-122.90579</v>
       </c>
-      <c r="K21" s="2">
+      <c r="M21" s="2">
         <v>162</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O21" s="1">
         <v>21</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O21" s="1" t="s">
+      <c r="P21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:18">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2304,35 +2449,41 @@
       <c r="F22" s="2">
         <v>-74.103797306100006</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="1">
         <v>37311</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="2">
+      <c r="K22" s="2">
         <v>43.696465000000003</v>
       </c>
-      <c r="J22" s="2">
+      <c r="L22" s="2">
         <v>-122.965873</v>
       </c>
-      <c r="K22" s="2">
+      <c r="M22" s="2">
         <v>265</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="1">
         <v>22</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O22" s="1" t="s">
+      <c r="P22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:18">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2348,35 +2499,41 @@
       <c r="F23" s="2">
         <v>12.4585005481</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" s="1">
         <v>37313</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I23" s="2">
+      <c r="K23" s="2">
         <v>44.028767999999999</v>
       </c>
-      <c r="J23" s="2">
+      <c r="L23" s="2">
         <v>-122.98994399999999</v>
       </c>
-      <c r="K23" s="2">
+      <c r="M23" s="2">
         <v>138</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" s="1">
         <v>23</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O23" s="1" t="s">
+      <c r="P23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:18">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2392,35 +2549,41 @@
       <c r="F24" s="2">
         <v>119.584524575</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="1">
         <v>37301</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="2">
+      <c r="K24" s="2">
         <v>43.831426</v>
       </c>
-      <c r="J24" s="2">
+      <c r="L24" s="2">
         <v>-122.997659</v>
       </c>
-      <c r="K24" s="2">
+      <c r="M24" s="2">
         <v>244</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" s="1">
-        <v>24</v>
-      </c>
       <c r="N24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O24" s="1">
+        <v>24</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:18">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2436,38 +2599,44 @@
       <c r="F25" s="2">
         <v>88.039357639000002</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" s="1">
         <v>37297</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="2">
+      <c r="K25" s="2">
         <v>43.926537000000003</v>
       </c>
-      <c r="J25" s="2">
+      <c r="L25" s="2">
         <v>-123.000882</v>
       </c>
-      <c r="K25" s="2">
+      <c r="M25" s="2">
         <v>163</v>
       </c>
-      <c r="L25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25" s="1">
+      <c r="N25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O25" s="1">
         <v>25</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R25" t="s">
         <v>139</v>
       </c>
-      <c r="P25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2483,35 +2652,41 @@
       <c r="F26" s="2">
         <v>-56.288383543400002</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" s="1">
         <v>26746</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I26" s="2">
+      <c r="K26" s="2">
         <v>43.778280000000002</v>
       </c>
-      <c r="J26" s="2">
+      <c r="L26" s="2">
         <v>-123.00539999999999</v>
       </c>
-      <c r="K26" s="2">
+      <c r="M26" s="2">
         <v>218</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26" s="1">
+      <c r="N26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O26" s="1">
         <v>26</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O26" s="1" t="s">
+      <c r="P26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:18">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2527,35 +2702,41 @@
       <c r="F27" s="2">
         <v>2.3402911085699998</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27" s="1">
         <v>37300</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="2">
+      <c r="K27" s="2">
         <v>43.836576000000001</v>
       </c>
-      <c r="J27" s="2">
+      <c r="L27" s="2">
         <v>-123.02488099999999</v>
       </c>
-      <c r="K27" s="2">
+      <c r="M27" s="2">
         <v>184</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" s="1">
-        <v>27</v>
-      </c>
       <c r="N27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="1">
+        <v>27</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:18">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2571,35 +2752,41 @@
       <c r="F28" s="2">
         <v>445.59622783899999</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" s="1">
         <v>18890</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I28" s="2">
+      <c r="K28" s="2">
         <v>43.922638999999997</v>
       </c>
-      <c r="J28" s="2">
+      <c r="L28" s="2">
         <v>-123.03447199999999</v>
       </c>
-      <c r="K28" s="2">
+      <c r="M28" s="2">
         <v>162</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" s="1">
+      <c r="N28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O28" s="1">
         <v>28</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:18">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2615,35 +2802,41 @@
       <c r="F29" s="2">
         <v>249.72867814899999</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" s="1">
         <v>11276</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I29" s="2">
+      <c r="K29" s="2">
         <v>43.809027999999998</v>
       </c>
-      <c r="J29" s="2">
+      <c r="L29" s="2">
         <v>-123.04774999999999</v>
       </c>
-      <c r="K29" s="2">
+      <c r="M29" s="2">
         <v>203</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" s="1">
+      <c r="N29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O29" s="1">
         <v>29</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O29" s="1" t="s">
+      <c r="P29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:18">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2656,35 +2849,41 @@
       <c r="E30" s="3">
         <v>6460.9740000000002</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30" s="1">
         <v>37293</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="2">
+      <c r="K30" s="2">
         <v>44.122377</v>
       </c>
-      <c r="J30" s="2">
+      <c r="L30" s="2">
         <v>-123.055148</v>
       </c>
-      <c r="K30" s="2">
+      <c r="M30" s="2">
         <v>122</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" s="1">
+      <c r="N30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O30" s="1">
         <v>30</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="P30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2697,35 +2896,41 @@
       <c r="E31" s="3">
         <v>6460.9740000000002</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I31" s="1">
         <v>37292</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I31" s="2">
+      <c r="K31" s="2">
         <v>44.144317000000001</v>
       </c>
-      <c r="J31" s="2">
+      <c r="L31" s="2">
         <v>-123.06054</v>
       </c>
-      <c r="K31" s="2">
+      <c r="M31" s="2">
         <v>120</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="1">
+      <c r="N31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O31" s="1">
         <v>31</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="P31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2738,35 +2943,41 @@
       <c r="E32" s="3">
         <v>0</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I32" s="1">
         <v>11288</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I32" s="2">
+      <c r="K32" s="2">
         <v>43.795555999999998</v>
       </c>
-      <c r="J32" s="2">
+      <c r="L32" s="2">
         <v>-123.06783299999999</v>
       </c>
-      <c r="K32" s="2">
+      <c r="M32" s="2">
         <v>196</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M32" s="1">
+      <c r="N32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O32" s="1">
         <v>32</v>
       </c>
-      <c r="N32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="P32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2782,35 +2993,41 @@
       <c r="F33" s="2">
         <v>-26.9799502977</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" s="1">
         <v>37295</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I33" s="2">
+      <c r="K33" s="2">
         <v>43.926825999999998</v>
       </c>
-      <c r="J33" s="2">
+      <c r="L33" s="2">
         <v>-123.069165</v>
       </c>
-      <c r="K33" s="2">
+      <c r="M33" s="2">
         <v>166</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M33" s="1">
+      <c r="N33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O33" s="1">
         <v>33</v>
       </c>
-      <c r="N33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q33" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:18">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2826,35 +3043,41 @@
       <c r="F34" s="2">
         <v>-394.62673809</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="1">
         <v>11277</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I34" s="2">
+      <c r="K34" s="2">
         <v>43.784582999999998</v>
       </c>
-      <c r="J34" s="2">
+      <c r="L34" s="2">
         <v>-123.069722</v>
       </c>
-      <c r="K34" s="2">
+      <c r="M34" s="2">
         <v>198</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34" s="1">
         <v>34</v>
       </c>
-      <c r="N34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q34" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:18">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2870,35 +3093,41 @@
       <c r="F35" s="2">
         <v>-128.44958394099999</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" s="1">
         <v>37294</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I35" s="2">
+      <c r="K35" s="2">
         <v>43.796495</v>
       </c>
-      <c r="J35" s="2">
+      <c r="L35" s="2">
         <v>-123.081312</v>
       </c>
-      <c r="K35" s="2">
+      <c r="M35" s="2">
         <v>201</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M35" s="1">
+      <c r="N35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" s="1">
         <v>35</v>
       </c>
-      <c r="N35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:18">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2914,35 +3143,41 @@
       <c r="F36" s="2">
         <v>2.1934398907300001</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="1">
         <v>37296</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I36" s="2">
+      <c r="K36" s="2">
         <v>43.915295999999998</v>
       </c>
-      <c r="J36" s="2">
+      <c r="L36" s="2">
         <v>-123.143168</v>
       </c>
-      <c r="K36" s="2">
+      <c r="M36" s="2">
         <v>189</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="1">
+      <c r="N36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="1">
         <v>36</v>
       </c>
-      <c r="N36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O36" s="1" t="s">
+      <c r="P36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q36" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:18">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2958,38 +3193,44 @@
       <c r="F37" s="2">
         <v>5001.0296941500001</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" s="1">
         <v>37306</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="I37" s="2">
+      <c r="K37" s="2">
         <v>44.214965999999997</v>
       </c>
-      <c r="J37" s="2">
+      <c r="L37" s="2">
         <v>-123.197574</v>
       </c>
-      <c r="K37" s="2">
+      <c r="M37" s="2">
         <v>100</v>
       </c>
-      <c r="L37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" s="1">
+      <c r="N37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O37" s="1">
         <v>37</v>
       </c>
-      <c r="N37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="P37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3005,38 +3246,44 @@
       <c r="F38" s="2">
         <v>3001.0243398299999</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38" s="1">
         <v>37307</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I38" s="2">
+      <c r="K38" s="2">
         <v>44.211866000000001</v>
       </c>
-      <c r="J38" s="2">
+      <c r="L38" s="2">
         <v>-123.204864</v>
       </c>
-      <c r="K38" s="2">
+      <c r="M38" s="2">
         <v>101</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="1">
+      <c r="N38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" s="1">
         <v>38</v>
       </c>
-      <c r="N38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="P38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3052,38 +3299,44 @@
       <c r="F39" s="2">
         <v>5661.6572234300002</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="1">
         <v>37303</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="I39" s="2">
+      <c r="K39" s="2">
         <v>44.229646000000002</v>
       </c>
-      <c r="J39" s="2">
+      <c r="L39" s="2">
         <v>-123.21160399999999</v>
       </c>
-      <c r="K39" s="2">
+      <c r="M39" s="2">
         <v>98</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" s="1">
+      <c r="N39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="1">
         <v>39</v>
       </c>
-      <c r="N39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="P39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3099,38 +3352,44 @@
       <c r="F40" s="2">
         <v>5324.0959771099997</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I40" s="1">
         <v>37305</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I40" s="2">
+      <c r="K40" s="2">
         <v>44.229785999999997</v>
       </c>
-      <c r="J40" s="2">
+      <c r="L40" s="2">
         <v>-123.213184</v>
       </c>
-      <c r="K40" s="2">
+      <c r="M40" s="2">
         <v>98</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M40" s="1">
+      <c r="N40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O40" s="1">
         <v>40</v>
       </c>
-      <c r="N40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="P40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3146,38 +3405,44 @@
       <c r="F41" s="2">
         <v>-3043.5151881699999</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I41" s="1">
         <v>37314</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I41" s="2">
+      <c r="K41" s="2">
         <v>44.040894999999999</v>
       </c>
-      <c r="J41" s="2">
+      <c r="L41" s="2">
         <v>-123.343457</v>
       </c>
-      <c r="K41" s="2">
+      <c r="M41" s="2">
         <v>126</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M41" s="1">
+      <c r="N41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O41" s="1">
         <v>41</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="P41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3193,38 +3458,44 @@
       <c r="F42" s="2">
         <v>-2356.1882818300001</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I42" s="1">
         <v>37315</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I42" s="2">
+      <c r="K42" s="2">
         <v>44.031995000000002</v>
       </c>
-      <c r="J42" s="2">
+      <c r="L42" s="2">
         <v>-123.352557</v>
       </c>
-      <c r="K42" s="2">
+      <c r="M42" s="2">
         <v>136</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42" s="1">
+      <c r="N42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" s="1">
         <v>42</v>
       </c>
-      <c r="N42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="P42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3240,35 +3511,41 @@
       <c r="F43" s="2">
         <v>-301.00860494199998</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I43" s="1">
         <v>36026</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I43" s="2">
+      <c r="K43" s="2">
         <v>45.818055999999999</v>
       </c>
-      <c r="J43" s="2">
+      <c r="L43" s="2">
         <v>-123.95138900000001</v>
       </c>
-      <c r="K43" s="2">
+      <c r="M43" s="2">
         <v>83</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="1">
+      <c r="N43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O43" s="1">
         <v>43</v>
       </c>
-      <c r="N43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O43" s="1" t="s">
+      <c r="P43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q43" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:18">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3284,38 +3561,44 @@
       <c r="F44" s="2">
         <v>1245.3863773800001</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I44" s="1">
         <v>36828</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I44" s="2">
+      <c r="K44" s="2">
         <v>43.580058999999999</v>
       </c>
-      <c r="J44" s="2">
+      <c r="L44" s="2">
         <v>-124.163275</v>
       </c>
-      <c r="K44" s="2">
+      <c r="M44" s="2">
         <v>5</v>
       </c>
-      <c r="L44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" s="1">
+      <c r="N44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O44" s="1">
         <v>44</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P44" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="P44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -3332,37 +3615,45 @@
       <c r="F45" s="1">
         <v>-57.639243999999998</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I45" s="1">
         <v>10671</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K45" s="2">
         <v>43.958750000000002</v>
       </c>
-      <c r="J45" s="2">
+      <c r="L45" s="2">
         <v>-122.808583</v>
       </c>
-      <c r="K45" s="1">
+      <c r="M45" s="1">
         <v>195</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" s="1">
+      <c r="N45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O45" s="1">
         <v>16</v>
       </c>
-      <c r="N45" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O45" t="s">
-        <v>148</v>
+      <c r="P45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P45">
-    <filterColumn colId="14"/>
+  <autoFilter ref="A1:R45">
+    <filterColumn colId="6"/>
+    <filterColumn colId="7"/>
+    <filterColumn colId="16"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3370,13 +3661,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C46" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3470,7 +3762,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" hidden="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3538,7 +3830,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3606,7 +3898,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" hidden="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3674,7 +3966,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" hidden="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3738,14 +4030,14 @@
       <c r="U5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>136</v>
+      <c r="V5" t="s">
+        <v>154</v>
       </c>
       <c r="W5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" hidden="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3813,7 +4105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" hidden="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3881,7 +4173,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" hidden="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3949,7 +4241,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" hidden="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4017,7 +4309,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" hidden="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4085,7 +4377,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" hidden="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4149,14 +4441,14 @@
       <c r="U11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" t="s">
+        <v>156</v>
+      </c>
+      <c r="W11" t="s">
         <v>136</v>
       </c>
-      <c r="W11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
+    </row>
+    <row r="12" spans="1:23" hidden="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4224,7 +4516,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" hidden="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4292,7 +4584,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" hidden="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4360,7 +4652,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" hidden="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4425,13 +4717,13 @@
         <v>27</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" hidden="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4496,13 +4788,13 @@
         <v>27</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" hidden="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4570,7 +4862,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" hidden="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4638,7 +4930,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" hidden="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4702,14 +4994,14 @@
       <c r="U19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>136</v>
+      <c r="V19" t="s">
+        <v>154</v>
       </c>
       <c r="W19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" hidden="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4777,7 +5069,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" hidden="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4845,7 +5137,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" hidden="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4913,7 +5205,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" hidden="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4981,7 +5273,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" hidden="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5049,7 +5341,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" hidden="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5114,13 +5406,13 @@
         <v>27</v>
       </c>
       <c r="V25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W25" t="s">
         <v>139</v>
       </c>
-      <c r="W25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
+    </row>
+    <row r="26" spans="1:23" hidden="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5188,7 +5480,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" hidden="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5256,7 +5548,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" hidden="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5324,7 +5616,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" hidden="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5392,7 +5684,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" hidden="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5454,10 +5746,10 @@
         <v>27</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" hidden="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5519,10 +5811,10 @@
         <v>27</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" hidden="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5584,10 +5876,10 @@
         <v>27</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" hidden="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5655,7 +5947,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" hidden="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5723,7 +6015,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" hidden="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5791,7 +6083,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" hidden="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5859,7 +6151,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" hidden="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5924,13 +6216,13 @@
         <v>27</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" hidden="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5995,13 +6287,13 @@
         <v>27</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" hidden="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6066,13 +6358,13 @@
         <v>27</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" hidden="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6137,13 +6429,13 @@
         <v>27</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" hidden="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6208,13 +6500,13 @@
         <v>27</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" hidden="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6279,13 +6571,13 @@
         <v>27</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" hidden="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6353,7 +6645,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" hidden="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6418,10 +6710,10 @@
         <v>27</v>
       </c>
       <c r="V44" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -6444,7 +6736,7 @@
         <v>10671</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H45" s="2">
         <v>43.958750000000002</v>
@@ -6486,13 +6778,20 @@
         <v>16</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="V45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V45">
+    <filterColumn colId="21">
+      <filters>
+        <filter val="Not Required"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6503,7 +6802,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W1048576"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6600,7 +6899,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6668,7 +6967,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" ht="15" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -6736,7 +7035,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" ht="15" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6868,14 +7167,14 @@
       <c r="U5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>136</v>
+      <c r="V5" t="s">
+        <v>154</v>
       </c>
       <c r="W5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6943,7 +7242,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" ht="15" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -7011,7 +7310,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" ht="15" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -7079,7 +7378,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" ht="15" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -7147,7 +7446,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" ht="15" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -7279,14 +7578,14 @@
       <c r="U11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" t="s">
+        <v>156</v>
+      </c>
+      <c r="W11" t="s">
         <v>136</v>
       </c>
-      <c r="W11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
+    </row>
+    <row r="12" spans="1:23" ht="15" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -7354,7 +7653,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" ht="15" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -7422,7 +7721,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" ht="15" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -7490,7 +7789,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" ht="15" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -7555,13 +7854,13 @@
         <v>27</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -7626,13 +7925,13 @@
         <v>27</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15" customHeight="1">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -7700,7 +7999,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" ht="15" customHeight="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -7832,14 +8131,14 @@
       <c r="U19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>136</v>
+      <c r="V19" t="s">
+        <v>154</v>
       </c>
       <c r="W19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -7907,7 +8206,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" ht="15" customHeight="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -7975,7 +8274,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" ht="15" customHeight="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -8043,7 +8342,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" ht="15" customHeight="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -8111,7 +8410,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" ht="15" customHeight="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -8179,7 +8478,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" ht="15" customHeight="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -8244,13 +8543,13 @@
         <v>27</v>
       </c>
       <c r="V25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W25" t="s">
         <v>139</v>
       </c>
-      <c r="W25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
+    </row>
+    <row r="26" spans="1:23" ht="15" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -8318,7 +8617,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" ht="15" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -8386,7 +8685,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" ht="15" customHeight="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -8454,7 +8753,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" ht="15" customHeight="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -8522,7 +8821,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" ht="15" customHeight="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -8585,10 +8884,10 @@
         <v>27</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="15" customHeight="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -8651,10 +8950,10 @@
         <v>27</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="15" customHeight="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -8717,10 +9016,10 @@
         <v>27</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="15" customHeight="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -8788,7 +9087,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" ht="15" customHeight="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -8856,7 +9155,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" ht="15" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -8924,7 +9223,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" ht="15" customHeight="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -8992,7 +9291,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" ht="15" customHeight="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -9057,13 +9356,13 @@
         <v>27</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="15" customHeight="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -9128,13 +9427,13 @@
         <v>27</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="15" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -9199,13 +9498,13 @@
         <v>27</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="15" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -9270,13 +9569,13 @@
         <v>27</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W40" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="15" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -9341,13 +9640,13 @@
         <v>27</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="15" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -9412,13 +9711,13 @@
         <v>27</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="15" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -9486,7 +9785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" ht="15" customHeight="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -9551,13 +9850,14 @@
         <v>27</v>
       </c>
       <c r="V44" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:W44"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
debugged estuary analysis script which uses 2010 stations to classify new stations.
</commit_message>
<xml_diff>
--- a/StationsToLocate/FinalList/Additional_LASAR_Stations.xlsx
+++ b/StationsToLocate/FinalList/Additional_LASAR_Stations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="161">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -454,9 +454,6 @@
   </si>
   <si>
     <t>Little Fall Creek</t>
-  </si>
-  <si>
-    <t>Reviewed</t>
   </si>
   <si>
     <t>Not Required</t>
@@ -1339,7 +1336,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1370,34 +1367,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>9</v>
@@ -1435,10 +1432,10 @@
         <v>32.265093441499999</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I2" s="1">
         <v>36445</v>
@@ -1485,10 +1482,10 @@
         <v>301.80591385700001</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I3" s="1">
         <v>12015</v>
@@ -1535,10 +1532,10 @@
         <v>581.89186180800004</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I4" s="1">
         <v>10708</v>
@@ -1585,10 +1582,10 @@
         <v>655.25162609200004</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I5" s="1">
         <v>34086</v>
@@ -1615,10 +1612,10 @@
         <v>27</v>
       </c>
       <c r="Q5" t="s">
+        <v>153</v>
+      </c>
+      <c r="R5" t="s">
         <v>154</v>
-      </c>
-      <c r="R5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -1638,10 +1635,10 @@
         <v>-419.08513926299997</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I6" s="1">
         <v>28010</v>
@@ -1688,10 +1685,10 @@
         <v>354.61531665400003</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I7" s="1">
         <v>28608</v>
@@ -1738,10 +1735,10 @@
         <v>-108.473015166</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I8" s="1">
         <v>10908</v>
@@ -1788,10 +1785,10 @@
         <v>-366.25276947200001</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I9" s="1">
         <v>37318</v>
@@ -1838,10 +1835,10 @@
         <v>120.319726907</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I10" s="1">
         <v>37317</v>
@@ -1888,10 +1885,10 @@
         <v>75.777605241700002</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I11" s="1">
         <v>10913</v>
@@ -1918,7 +1915,7 @@
         <v>27</v>
       </c>
       <c r="Q11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R11" t="s">
         <v>136</v>
@@ -1941,10 +1938,10 @@
         <v>204.27260615500001</v>
       </c>
       <c r="G12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I12" s="1">
         <v>10668</v>
@@ -1991,10 +1988,10 @@
         <v>163.02957825799999</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I13" s="1">
         <v>11375</v>
@@ -2041,10 +2038,10 @@
         <v>35.990392590299997</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I14" s="1">
         <v>37308</v>
@@ -2091,10 +2088,10 @@
         <v>4914.3600231999999</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I15" s="1">
         <v>37310</v>
@@ -2144,10 +2141,10 @@
         <v>2857.6041715400002</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I16" s="1">
         <v>37309</v>
@@ -2197,10 +2194,10 @@
         <v>163.39601961899999</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I17" s="1">
         <v>37312</v>
@@ -2247,10 +2244,10 @@
         <v>42.778447677700001</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I18" s="1">
         <v>37299</v>
@@ -2297,10 +2294,10 @@
         <v>1670.9214633199999</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I19" s="1">
         <v>35348</v>
@@ -2327,10 +2324,10 @@
         <v>27</v>
       </c>
       <c r="Q19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2350,10 +2347,10 @@
         <v>54.1944730142</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I20" s="1">
         <v>37302</v>
@@ -2400,10 +2397,10 @@
         <v>73.680022717900002</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I21" s="1">
         <v>37316</v>
@@ -2450,10 +2447,10 @@
         <v>-74.103797306100006</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I22" s="1">
         <v>37311</v>
@@ -2500,10 +2497,10 @@
         <v>12.4585005481</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I23" s="1">
         <v>37313</v>
@@ -2550,10 +2547,10 @@
         <v>119.584524575</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I24" s="1">
         <v>37301</v>
@@ -2600,10 +2597,10 @@
         <v>88.039357639000002</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I25" s="1">
         <v>37297</v>
@@ -2653,10 +2650,10 @@
         <v>-56.288383543400002</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I26" s="1">
         <v>26746</v>
@@ -2703,10 +2700,10 @@
         <v>2.3402911085699998</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I27" s="1">
         <v>37300</v>
@@ -2753,10 +2750,10 @@
         <v>445.59622783899999</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I28" s="1">
         <v>18890</v>
@@ -2803,10 +2800,10 @@
         <v>249.72867814899999</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I29" s="1">
         <v>11276</v>
@@ -2850,10 +2847,10 @@
         <v>6460.9740000000002</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I30" s="1">
         <v>37293</v>
@@ -2897,10 +2894,10 @@
         <v>6460.9740000000002</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I31" s="1">
         <v>37292</v>
@@ -2944,10 +2941,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I32" s="1">
         <v>11288</v>
@@ -2994,10 +2991,10 @@
         <v>-26.9799502977</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I33" s="1">
         <v>37295</v>
@@ -3044,10 +3041,10 @@
         <v>-394.62673809</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I34" s="1">
         <v>11277</v>
@@ -3094,10 +3091,10 @@
         <v>-128.44958394099999</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I35" s="1">
         <v>37294</v>
@@ -3144,10 +3141,10 @@
         <v>2.1934398907300001</v>
       </c>
       <c r="G36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I36" s="1">
         <v>37296</v>
@@ -3194,10 +3191,10 @@
         <v>5001.0296941500001</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I37" s="1">
         <v>37306</v>
@@ -3247,10 +3244,10 @@
         <v>3001.0243398299999</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I38" s="1">
         <v>37307</v>
@@ -3300,10 +3297,10 @@
         <v>5661.6572234300002</v>
       </c>
       <c r="G39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I39" s="1">
         <v>37303</v>
@@ -3353,10 +3350,10 @@
         <v>5324.0959771099997</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I40" s="1">
         <v>37305</v>
@@ -3406,10 +3403,10 @@
         <v>-3043.5151881699999</v>
       </c>
       <c r="G41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I41" s="1">
         <v>37314</v>
@@ -3459,10 +3456,10 @@
         <v>-2356.1882818300001</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I42" s="1">
         <v>37315</v>
@@ -3512,10 +3509,10 @@
         <v>-301.00860494199998</v>
       </c>
       <c r="G43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I43" s="1">
         <v>36026</v>
@@ -3562,10 +3559,10 @@
         <v>1245.3863773800001</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I44" s="1">
         <v>36828</v>
@@ -3616,10 +3613,10 @@
         <v>-57.639243999999998</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="I45" s="1">
         <v>10671</v>
@@ -3643,10 +3640,10 @@
         <v>16</v>
       </c>
       <c r="P45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q45" t="s">
         <v>144</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -3661,14 +3658,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
+      <selection pane="bottomRight" activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3762,7 +3758,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3830,7 +3826,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1">
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3898,7 +3894,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1">
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3966,7 +3962,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1">
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4031,13 +4027,13 @@
         <v>27</v>
       </c>
       <c r="V5" t="s">
+        <v>153</v>
+      </c>
+      <c r="W5" t="s">
         <v>154</v>
       </c>
-      <c r="W5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" hidden="1">
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4105,7 +4101,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:23" hidden="1">
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4173,7 +4169,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:23" hidden="1">
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4241,7 +4237,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:23" hidden="1">
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4309,7 +4305,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:23" hidden="1">
+    <row r="10" spans="1:23">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4377,7 +4373,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:23" hidden="1">
+    <row r="11" spans="1:23">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4442,13 +4438,13 @@
         <v>27</v>
       </c>
       <c r="V11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:23" hidden="1">
+    <row r="12" spans="1:23">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4516,7 +4512,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:23" hidden="1">
+    <row r="13" spans="1:23">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4584,7 +4580,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:23" hidden="1">
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4652,7 +4648,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:23" hidden="1">
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4723,7 +4719,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:23" hidden="1">
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4794,7 +4790,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:23" hidden="1">
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4862,7 +4858,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:23" hidden="1">
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4930,7 +4926,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:23" hidden="1">
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4995,13 +4991,13 @@
         <v>27</v>
       </c>
       <c r="V19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" hidden="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5069,7 +5065,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:23" hidden="1">
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5137,7 +5133,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:23" hidden="1">
+    <row r="22" spans="1:23">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5205,7 +5201,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:23" hidden="1">
+    <row r="23" spans="1:23">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5273,7 +5269,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:23" hidden="1">
+    <row r="24" spans="1:23">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5341,7 +5337,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="1:23" hidden="1">
+    <row r="25" spans="1:23">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5412,7 +5408,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:23" hidden="1">
+    <row r="26" spans="1:23">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5480,7 +5476,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:23" hidden="1">
+    <row r="27" spans="1:23">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5548,7 +5544,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:23" hidden="1">
+    <row r="28" spans="1:23">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5616,7 +5612,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:23" hidden="1">
+    <row r="29" spans="1:23">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5684,7 +5680,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:23" hidden="1">
+    <row r="30" spans="1:23">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5749,7 +5745,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:23" hidden="1">
+    <row r="31" spans="1:23">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5814,7 +5810,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:23" hidden="1">
+    <row r="32" spans="1:23">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5879,7 +5875,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:23" hidden="1">
+    <row r="33" spans="1:23">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5947,7 +5943,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:23" hidden="1">
+    <row r="34" spans="1:23">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -6015,7 +6011,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:23" hidden="1">
+    <row r="35" spans="1:23">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -6083,7 +6079,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:23" hidden="1">
+    <row r="36" spans="1:23">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -6151,7 +6147,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:23" hidden="1">
+    <row r="37" spans="1:23">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -6222,7 +6218,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:23" hidden="1">
+    <row r="38" spans="1:23">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -6293,7 +6289,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:23" hidden="1">
+    <row r="39" spans="1:23">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -6364,7 +6360,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:23" hidden="1">
+    <row r="40" spans="1:23">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6435,7 +6431,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:23" hidden="1">
+    <row r="41" spans="1:23">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6506,7 +6502,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:23" hidden="1">
+    <row r="42" spans="1:23">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6577,7 +6573,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:23" hidden="1">
+    <row r="43" spans="1:23">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6645,7 +6641,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:23" hidden="1">
+    <row r="44" spans="1:23">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6778,19 +6774,15 @@
         <v>16</v>
       </c>
       <c r="U45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="V45" t="s">
         <v>144</v>
-      </c>
-      <c r="V45" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:V45">
-    <filterColumn colId="21">
-      <filters>
-        <filter val="Not Required"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="21"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6801,7 +6793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
@@ -7168,10 +7160,10 @@
         <v>27</v>
       </c>
       <c r="V5" t="s">
+        <v>153</v>
+      </c>
+      <c r="W5" t="s">
         <v>154</v>
-      </c>
-      <c r="W5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1">
@@ -7579,7 +7571,7 @@
         <v>27</v>
       </c>
       <c r="V11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W11" t="s">
         <v>136</v>
@@ -8132,10 +8124,10 @@
         <v>27</v>
       </c>
       <c r="V19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1">

</xml_diff>